<commit_message>
fix: Correct Scheme P lunch hours and 7-day threshold per MOM guidelines
- Added pattern-specific lunch rules for Scheme P:
  * ≤4 days: 1.00h lunch (for shifts > 6h)
  * 5 days: 0.75h lunch (for shifts > 6h)
  * ≥6 days: 0.00h lunch (no lunch break)
- Changed 7-day threshold from 4.283h to 4.0h per official table
- Verified all calculations match MOM Scheme P guidelines exactly:
  * 4 days: 8.0h normal + 0.0h OT ✓
  * 5 days: 6.0h normal + 2.25h OT ✓
  * 6 days: 5.0h normal + 3.0h OT ✓
  * 7 days: 4.0h normal + 4.0h OT ✓
- Scheme A/B calculations remain completely unaffected
</commit_message>
<xml_diff>
--- a/Monthly Hours Calculation.xlsx
+++ b/Monthly Hours Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glori/1 Anthony_Workspace/My Developments/NGRS/ngrs-solver-v0.7/ngrssolver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD2FC1D6-2ACE-3741-BC8E-29A6278E9E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2499A37D-B6F7-0A4E-812A-072DA6089880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29920" windowHeight="18680" xr2:uid="{3D69C63B-0B6D-7744-8791-C3F4702C993F}"/>
   </bookViews>
@@ -858,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21D1D11-0A7A-9F4F-80FB-42FB3F525BF2}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>